<commit_message>
Made changes for tests
Made changes to the program and files in order to perform tests
</commit_message>
<xml_diff>
--- a/Game_Engine/Shared/Resources/maps/maps.xlsx
+++ b/Game_Engine/Shared/Resources/maps/maps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="8">
   <si>
     <t>MapID</t>
   </si>
@@ -378,8 +378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1488,6 +1488,9 @@
       <c r="C79">
         <v>9</v>
       </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="80" spans="1:4" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
@@ -1498,6 +1501,9 @@
       </c>
       <c r="C80" s="2">
         <v>9</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>